<commit_message>
completed txt files grading
</commit_message>
<xml_diff>
--- a/app/media/word_lists/word_lists.xlsx
+++ b/app/media/word_lists/word_lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\little\Desktop\little\vlad\Work\emerson\demo\app\source_code\TextReviewer\word_lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\little\Desktop\little\vlad\Work\emerson\Draft1\source_code\eng-txt-grader\app\media\word_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CD96D2-6A6B-4137-A135-8525613F4DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125F9883-8BA6-4B76-9DA7-C3A60EBDFA8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kindergarten" sheetId="3" r:id="rId1"/>
@@ -3801,7 +3801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A115"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A79" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4890,7 +4890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -5253,7 +5255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K776"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>